<commit_message>
Add support for expected test cases data frame serialization in csv and json. Now the expected data frame can loaded from an "expected" xlsx, csv or json file.
</commit_message>
<xml_diff>
--- a/tests/integration_cases/expected/test_case6.xlsx
+++ b/tests/integration_cases/expected/test_case6.xlsx
@@ -50,10 +50,10 @@
     <t>PIBpm - Producto Interno Bruto a precios de mercado - VABpb - Valor Agregado Bruto a precios basicos - K - ACTIVIDADES INMOBILIARIAS, EMPRESARIALES Y DE ALQUILER</t>
   </si>
   <si>
-    <t>PIBpm - Producto Interno Bruto a precios de mercado - VABpb - Valor Agregado Bruto a precios basicos - L - ADMINISTRACION PÚBLICA Y DEFENSA; PLANES DE SEGURIDAD SOCIAL DE AFILIACION OBLIGATORIA</t>
+    <t>PIBpm - Producto Interno Bruto a precios de mercado - VABpb - Valor Agregado Bruto a precios basicos - L - ADMINISTRACION PUBLICA Y DEFENSA; PLANES DE SEGURIDAD SOCIAL DE AFILIACION OBLIGATORIA</t>
   </si>
   <si>
-    <t>PIBpm - Producto Interno Bruto a precios de mercado - VABpb - Valor Agregado Bruto a precios basicos - M - ENSEÑANZA</t>
+    <t>PIBpm - Producto Interno Bruto a precios de mercado - VABpb - Valor Agregado Bruto a precios basicos - M - ENSENANZA</t>
   </si>
   <si>
     <t>PIBpm - Producto Interno Bruto a precios de mercado - VABpb - Valor Agregado Bruto a precios basicos - N - SERVICIOS SOCIALES Y DE SALUD</t>
@@ -87,7 +87,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -99,12 +99,17 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Verdana"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -151,19 +156,19 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="4" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">

</xml_diff>